<commit_message>
Loan Provisioning 10 test cases
</commit_message>
<xml_diff>
--- a/Mifos Automation Excels/Client/2480-RBI-EI-DB-SAR-REC-NOCOM-RNI-CTPD-SAR-MD-TR-2-DATE-VAR-INST-UPFRONT-Makerepayment2.xlsx
+++ b/Mifos Automation Excels/Client/2480-RBI-EI-DB-SAR-REC-NOCOM-RNI-CTPD-SAR-MD-TR-2-DATE-VAR-INST-UPFRONT-Makerepayment2.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\mifosx-e2e-testing\Mifos Automation Excels\Client\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="7755" tabRatio="696" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="7755" tabRatio="696" firstSheet="3" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="5" r:id="rId1"/>
@@ -22,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="58">
   <si>
     <t>#</t>
   </si>
@@ -165,9 +170,6 @@
     <t>$ 5,000</t>
   </si>
   <si>
-    <t>system</t>
-  </si>
-  <si>
     <t>Interest Receivable(3)</t>
   </si>
   <si>
@@ -195,23 +197,17 @@
     <t>$ 25</t>
   </si>
   <si>
-    <t>L54</t>
-  </si>
-  <si>
-    <t>L55</t>
-  </si>
-  <si>
-    <t>L58</t>
-  </si>
-  <si>
-    <t>$ 83.23</t>
+    <t>L50</t>
+  </si>
+  <si>
+    <t>$ 560.09</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -221,6 +217,14 @@
     </font>
     <font>
       <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -305,7 +309,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -349,36 +353,49 @@
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -427,7 +444,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -460,9 +477,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -495,6 +529,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1490,8 +1541,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1654,7 +1705,7 @@
         <v>42005</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E5" s="6">
         <v>560.09</v>
@@ -1886,7 +1937,7 @@
         <v>42050</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E2" s="16" t="s">
         <v>31</v>
@@ -1899,7 +1950,7 @@
       </c>
       <c r="H2" s="15"/>
       <c r="I2" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1913,7 +1964,7 @@
         <v>42050</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E3" s="16" t="s">
         <v>31</v>
@@ -1922,11 +1973,11 @@
         <v>30</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H3" s="15"/>
       <c r="I3" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1940,7 +1991,7 @@
         <v>42050</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E4" s="16" t="s">
         <v>31</v>
@@ -1952,7 +2003,7 @@
         <v>32</v>
       </c>
       <c r="H4" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I4" s="15"/>
     </row>
@@ -1966,7 +2017,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:I1"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2061,9 +2112,6 @@
         <v>32</v>
       </c>
       <c r="H3" s="13"/>
-      <c r="I3" s="13" t="s">
-        <v>46</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2075,7 +2123,7 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2132,7 +2180,7 @@
         <v>42064</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E2" s="19" t="s">
         <v>31</v>
@@ -2145,7 +2193,7 @@
       </c>
       <c r="H2" s="18"/>
       <c r="I2" s="19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -2159,7 +2207,7 @@
         <v>42064</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E3" s="19" t="s">
         <v>31</v>
@@ -2168,11 +2216,11 @@
         <v>30</v>
       </c>
       <c r="G3" s="19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H3" s="18"/>
       <c r="I3" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -2186,7 +2234,7 @@
         <v>42064</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E4" s="19" t="s">
         <v>31</v>
@@ -2198,7 +2246,7 @@
         <v>32</v>
       </c>
       <c r="H4" s="19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I4" s="18"/>
     </row>
@@ -2209,10 +2257,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2224,29 +2272,28 @@
     <col min="5" max="5" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="21" t="s">
         <v>27</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -2257,165 +2304,57 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="22">
-        <v>116</v>
-      </c>
-      <c r="B2" s="22" t="s">
+      <c r="A2" s="6">
+        <v>135</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="23">
-        <v>42050</v>
-      </c>
-      <c r="D2" s="22" t="s">
+      <c r="C2" s="7">
+        <v>42005</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="H2" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="E2" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="F2" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="G2" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="H2" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="I2" s="21"/>
+      <c r="I2" s="18"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="22">
-        <v>117</v>
-      </c>
-      <c r="B3" s="22" t="s">
+      <c r="A3" s="6">
+        <v>136</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="23">
-        <v>42050</v>
-      </c>
-      <c r="D3" s="22" t="s">
+      <c r="C3" s="7">
+        <v>42005</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" s="18"/>
+      <c r="I3" s="19" t="s">
         <v>57</v>
-      </c>
-      <c r="E3" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="F3" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="G3" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="H3" s="21"/>
-      <c r="I3" s="22" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="25">
-        <v>118</v>
-      </c>
-      <c r="B5" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="26">
-        <v>42064</v>
-      </c>
-      <c r="D5" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="E5" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="F5" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="G5" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="H5" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="I5" s="24"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="25">
-        <v>119</v>
-      </c>
-      <c r="B6" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="26">
-        <v>42064</v>
-      </c>
-      <c r="D6" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="E6" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="F6" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="G6" s="25" t="s">
-        <v>36</v>
-      </c>
-      <c r="H6" s="24"/>
-      <c r="I6" s="25" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="28">
-        <v>127</v>
-      </c>
-      <c r="B8" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="29">
-        <v>42095</v>
-      </c>
-      <c r="D8" s="28" t="s">
-        <v>59</v>
-      </c>
-      <c r="E8" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="F8" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="G8" s="28" t="s">
-        <v>48</v>
-      </c>
-      <c r="H8" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="I8" s="27"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="28">
-        <v>128</v>
-      </c>
-      <c r="B9" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="29">
-        <v>42095</v>
-      </c>
-      <c r="D9" s="28" t="s">
-        <v>59</v>
-      </c>
-      <c r="E9" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="F9" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="G9" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="H9" s="27"/>
-      <c r="I9" s="28" t="s">
-        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>